<commit_message>
Feat: Se finalizan los gráficos de matrimonios y fecundidad.
</commit_message>
<xml_diff>
--- a/Informe Demográfico/Matrimonios 2023.xlsx
+++ b/Informe Demográfico/Matrimonios 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182b438ead67ba54/Documentos/TABATA/Pensiones I/Informes/Informe-1-Pensiones/Informe Demográfico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{890F11B3-0587-4025-A489-776EBC003D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAA3C593-1912-47EF-A17F-68D8FAD47808}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{890F11B3-0587-4025-A489-776EBC003D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84CAD0A8-0FDB-4C58-B668-613200951C53}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Índice " sheetId="17" r:id="rId1"/>
@@ -2225,6 +2225,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -4494,6 +4498,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H6:H8"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="L6:L8"/>
@@ -4510,7 +4515,6 @@
     <mergeCell ref="N5:N8"/>
     <mergeCell ref="O5:O8"/>
     <mergeCell ref="G6:G8"/>
-    <mergeCell ref="H6:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.5" top="1.3" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4522,7 +4526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
@@ -7250,9 +7254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.4609375" defaultRowHeight="16.25" customHeight="1"/>
@@ -7295,10 +7299,10 @@
         <v>153</v>
       </c>
       <c r="F4" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="99" t="s">
         <v>154</v>
-      </c>
-      <c r="G4" s="99" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14">

</xml_diff>